<commit_message>
reviews saved on the bank
</commit_message>
<xml_diff>
--- a/reviews/review_bank.xlsx
+++ b/reviews/review_bank.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="159">
   <si>
     <t>Query</t>
   </si>
@@ -58,36 +58,87 @@
     <t>what can I make for a romantic dinner</t>
   </si>
   <si>
+    <t>amazing lavender crme brle</t>
+  </si>
+  <si>
+    <t>brled mashed sweet potatoes</t>
+  </si>
+  <si>
     <t>coffee brandy cream brulee</t>
   </si>
   <si>
+    <t>cream brulee with strawberries</t>
+  </si>
+  <si>
+    <t>cream cheese ice cream</t>
+  </si>
+  <si>
     <t>creme brulee for two</t>
   </si>
   <si>
+    <t>creme brulee pie</t>
+  </si>
+  <si>
     <t>easy creme brulee</t>
   </si>
   <si>
+    <t>instant peach brle</t>
+  </si>
+  <si>
     <t>lavender creme brulee</t>
   </si>
   <si>
     <t>no fail creme brulee</t>
   </si>
   <si>
+    <t>perfect creme brulee</t>
+  </si>
+  <si>
+    <t>pumpkin creme brulee</t>
+  </si>
+  <si>
+    <t>whiskey crme brle</t>
+  </si>
+  <si>
     <t>authentic bolognese sauce  sugo alla bolognese</t>
   </si>
   <si>
     <t>bolognese</t>
   </si>
   <si>
+    <t>incredible lasagna w  bolognese sauce</t>
+  </si>
+  <si>
+    <t>kelly s spaghetti bolognese</t>
+  </si>
+  <si>
+    <t>pumpkin bolognese</t>
+  </si>
+  <si>
+    <t>red wine bolognese</t>
+  </si>
+  <si>
     <t>spaghetti bolognese vegetarian</t>
   </si>
   <si>
+    <t>susan s delicious lasagna bolognese</t>
+  </si>
+  <si>
     <t>vegan bolognese</t>
   </si>
   <si>
     <t>vegan creamy spaghetti bolognese</t>
   </si>
   <si>
+    <t>all american apple pie spread</t>
+  </si>
+  <si>
+    <t>apple cranberry pie</t>
+  </si>
+  <si>
+    <t>apple gingersnap pie</t>
+  </si>
+  <si>
     <t>apple pie  1</t>
   </si>
   <si>
@@ -97,9 +148,27 @@
     <t>apple pie with a crust</t>
   </si>
   <si>
+    <t>apple pie with cheese sandwich</t>
+  </si>
+  <si>
+    <t>apple praline pie</t>
+  </si>
+  <si>
     <t>bread pudding apple pie</t>
   </si>
   <si>
+    <t>country apple crisp pie</t>
+  </si>
+  <si>
+    <t>crazy crust apple pie</t>
+  </si>
+  <si>
+    <t>crunchy caramel apple pie</t>
+  </si>
+  <si>
+    <t>crustless apple pie</t>
+  </si>
+  <si>
     <t>sheila s apple pie</t>
   </si>
   <si>
@@ -109,33 +178,105 @@
     <t>chocolate  cake</t>
   </si>
   <si>
+    <t>chocolate  chocolate  chocolate  bundt cake with chocolate glaze</t>
+  </si>
+  <si>
+    <t>chocolate chocolate cake</t>
+  </si>
+  <si>
+    <t>chocolate chocolate cake  bundt cake</t>
+  </si>
+  <si>
+    <t>chocolate chocolate chocolate bundt cake</t>
+  </si>
+  <si>
+    <t>chocolate idiot cake  flourless chocolate cake</t>
+  </si>
+  <si>
+    <t>death by chocolate cake aka chocolate heaven cake</t>
+  </si>
+  <si>
     <t>delicious chocolate cake</t>
   </si>
   <si>
+    <t>easy chocolate chocolate chip cake</t>
+  </si>
+  <si>
+    <t>german chocolate cake with milk chocolate ganache</t>
+  </si>
+  <si>
+    <t>great chocolate cake</t>
+  </si>
+  <si>
     <t>most chocolatey chocolate cake</t>
   </si>
   <si>
     <t>the best chocolate cake</t>
   </si>
   <si>
+    <t>basil lemonade</t>
+  </si>
+  <si>
+    <t>fresh lemonade syrup</t>
+  </si>
+  <si>
     <t>fresh minted lemonade</t>
   </si>
   <si>
     <t>fresh raspberry lemonade</t>
   </si>
   <si>
+    <t>grilled lemonade chicken</t>
+  </si>
+  <si>
+    <t>lemonade 6 ways</t>
+  </si>
+  <si>
+    <t>lemonade concentrate</t>
+  </si>
+  <si>
+    <t>lemonade smoothies</t>
+  </si>
+  <si>
     <t>most refreshing lemonade you will ever taste    quick   easy</t>
   </si>
   <si>
     <t>old fashioned  fresh lemonade</t>
   </si>
   <si>
+    <t>raspberry mint lemonade</t>
+  </si>
+  <si>
+    <t>rosemary lemonade</t>
+  </si>
+  <si>
+    <t>breakfast sandwich  quick   healthy</t>
+  </si>
+  <si>
     <t>healthy  quick  easy breakfast</t>
   </si>
   <si>
     <t>quick   easy low cal breakfast or lunch</t>
   </si>
   <si>
+    <t>quick and healthy black bean quesadillas</t>
+  </si>
+  <si>
+    <t>quick and healthy sweet potato lunch</t>
+  </si>
+  <si>
+    <t>quick bean salad</t>
+  </si>
+  <si>
+    <t>quick chickpea salad</t>
+  </si>
+  <si>
+    <t>quick clam chowder</t>
+  </si>
+  <si>
+    <t>quick healthy tasty breakfast</t>
+  </si>
+  <si>
     <t>quick rice sandwich</t>
   </si>
   <si>
@@ -145,42 +286,105 @@
     <t>two tin lunch</t>
   </si>
   <si>
+    <t>crispy tortilla pizza</t>
+  </si>
+  <si>
     <t>easy no yeast pizza dough</t>
   </si>
   <si>
+    <t>gluten free low carb pizza</t>
+  </si>
+  <si>
+    <t>greek mediterranean pizza</t>
+  </si>
+  <si>
+    <t>how to make pizza</t>
+  </si>
+  <si>
+    <t>individual pizzas</t>
+  </si>
+  <si>
+    <t>margherita pizza   white pizza</t>
+  </si>
+  <si>
     <t>no yeast homemade pizza</t>
   </si>
   <si>
+    <t>pizza con le patate  potato pizza</t>
+  </si>
+  <si>
     <t>pizza dough  with no yeast</t>
   </si>
   <si>
+    <t>pizza stuffed pizza</t>
+  </si>
+  <si>
     <t>pizza without the red sauce</t>
   </si>
   <si>
     <t>rice pizza</t>
   </si>
   <si>
+    <t>skinny pizza</t>
+  </si>
+  <si>
     <t>absolutely guilt free lazy morning pancakes</t>
   </si>
   <si>
+    <t>almond milk pancakes</t>
+  </si>
+  <si>
     <t>chinese pancakes   no egg or milk</t>
   </si>
   <si>
+    <t>chocolate pancake</t>
+  </si>
+  <si>
+    <t>easy morning pancakes</t>
+  </si>
+  <si>
     <t>fat free pancake</t>
   </si>
   <si>
+    <t>german pancake</t>
+  </si>
+  <si>
     <t>milk free  egg free pancakes</t>
   </si>
   <si>
+    <t>oma s oven pancake</t>
+  </si>
+  <si>
+    <t>packed pancakes</t>
+  </si>
+  <si>
     <t>pancakes   milk free</t>
   </si>
   <si>
+    <t>polish apple pancakes</t>
+  </si>
+  <si>
+    <t>spelt pancakes</t>
+  </si>
+  <si>
+    <t>the original pancake house apple pancake</t>
+  </si>
+  <si>
+    <t>washington retail pancake mix</t>
+  </si>
+  <si>
     <t>basic pasta dough  no egg</t>
   </si>
   <si>
     <t>breakfast pasta</t>
   </si>
   <si>
+    <t>cilantro lime pasta salad  with or without chicken</t>
+  </si>
+  <si>
+    <t>easy pasta and vegetables</t>
+  </si>
+  <si>
     <t>eggless pasta</t>
   </si>
   <si>
@@ -190,6 +394,30 @@
     <t>homemade  fat free  pasta</t>
   </si>
   <si>
+    <t>lucy s pasta</t>
+  </si>
+  <si>
+    <t>malfatti or gnocchi gnudi  pasta without the pasta</t>
+  </si>
+  <si>
+    <t>pasta omelette</t>
+  </si>
+  <si>
+    <t>pasta with asparagus and fried eggs</t>
+  </si>
+  <si>
+    <t>pasta with carbonara sauce</t>
+  </si>
+  <si>
+    <t>sauerkraut cake without eggs</t>
+  </si>
+  <si>
+    <t>simple savory pasta</t>
+  </si>
+  <si>
+    <t>whole wheat pasta noodles</t>
+  </si>
+  <si>
     <t>beef and rice stroganoff</t>
   </si>
   <si>
@@ -199,25 +427,70 @@
     <t>brazilian style beef strogonoff</t>
   </si>
   <si>
+    <t>chinese take out white rice</t>
+  </si>
+  <si>
+    <t>meatball stroganoff</t>
+  </si>
+  <si>
+    <t>mexican spiced rice</t>
+  </si>
+  <si>
+    <t>orange rice   rice cooker</t>
+  </si>
+  <si>
+    <t>quick home made rice better than rice a roni</t>
+  </si>
+  <si>
+    <t>rice cooker green rice</t>
+  </si>
+  <si>
+    <t>rice cooker wild rice</t>
+  </si>
+  <si>
     <t>sopa de pollo con arroz  chicken and rice soup</t>
   </si>
   <si>
     <t>sopa seca de arroz  mexican rice</t>
   </si>
   <si>
+    <t>better than sex chocolate sauce</t>
+  </si>
+  <si>
+    <t>cheesecake covered strawberries</t>
+  </si>
+  <si>
+    <t>french country chicken</t>
+  </si>
+  <si>
     <t>mirj s apres pta chicken dinner</t>
   </si>
   <si>
+    <t>mom what s for dinner pasta</t>
+  </si>
+  <si>
+    <t>romantic chicken roulades</t>
+  </si>
+  <si>
     <t>romantic chicken scallopine with saffron cream sauce</t>
   </si>
   <si>
+    <t>romantic pear dessert</t>
+  </si>
+  <si>
     <t>romantic stuffed chicken breasts a deux</t>
   </si>
   <si>
+    <t>romantic wild rice salad</t>
+  </si>
+  <si>
     <t>sensual chicken with champagne</t>
   </si>
   <si>
     <t>valentines day recipe</t>
+  </si>
+  <si>
+    <t>what a peasing salad</t>
   </si>
 </sst>
 </file>
@@ -575,7 +848,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C56"/>
+  <dimension ref="A1:C148"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -600,7 +873,7 @@
         <v>14</v>
       </c>
       <c r="C2">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -611,7 +884,7 @@
         <v>15</v>
       </c>
       <c r="C3">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -622,7 +895,7 @@
         <v>16</v>
       </c>
       <c r="C4">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -633,7 +906,7 @@
         <v>17</v>
       </c>
       <c r="C5">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -644,100 +917,100 @@
         <v>18</v>
       </c>
       <c r="C6">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B7" t="s">
         <v>19</v>
       </c>
       <c r="C7">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B8" t="s">
         <v>20</v>
       </c>
       <c r="C8">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B9" t="s">
         <v>21</v>
       </c>
       <c r="C9">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B10" t="s">
         <v>22</v>
       </c>
       <c r="C10">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B11" t="s">
         <v>23</v>
       </c>
       <c r="C11">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B12" t="s">
         <v>24</v>
       </c>
       <c r="C12">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="13" spans="1:3">
       <c r="A13" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B13" t="s">
         <v>25</v>
       </c>
       <c r="C13">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="14" spans="1:3">
       <c r="A14" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B14" t="s">
         <v>26</v>
       </c>
       <c r="C14">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="15" spans="1:3">
       <c r="A15" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B15" t="s">
         <v>27</v>
@@ -748,109 +1021,109 @@
     </row>
     <row r="16" spans="1:3">
       <c r="A16" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B16" t="s">
         <v>28</v>
       </c>
       <c r="C16">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B17" t="s">
         <v>29</v>
       </c>
       <c r="C17">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B18" t="s">
         <v>30</v>
       </c>
       <c r="C18">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:3">
       <c r="A19" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B19" t="s">
         <v>31</v>
       </c>
       <c r="C19">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:3">
       <c r="A20" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B20" t="s">
         <v>32</v>
       </c>
       <c r="C20">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:3">
       <c r="A21" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B21" t="s">
         <v>33</v>
       </c>
       <c r="C21">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:3">
       <c r="A22" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B22" t="s">
-        <v>7</v>
+        <v>34</v>
       </c>
       <c r="C22">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="23" spans="1:3">
       <c r="A23" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B23" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C23">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:3">
       <c r="A24" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B24" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C24">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="25" spans="1:3">
       <c r="A25" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B25" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C25">
         <v>4</v>
@@ -858,51 +1131,51 @@
     </row>
     <row r="26" spans="1:3">
       <c r="A26" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B26" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C26">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="27" spans="1:3">
       <c r="A27" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B27" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C27">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="28" spans="1:3">
       <c r="A28" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B28" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C28">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="29" spans="1:3">
       <c r="A29" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B29" t="s">
-        <v>40</v>
+        <v>5</v>
       </c>
       <c r="C29">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="30" spans="1:3">
       <c r="A30" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B30" t="s">
         <v>41</v>
@@ -913,7 +1186,7 @@
     </row>
     <row r="31" spans="1:3">
       <c r="A31" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B31" t="s">
         <v>42</v>
@@ -924,7 +1197,7 @@
     </row>
     <row r="32" spans="1:3">
       <c r="A32" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B32" t="s">
         <v>43</v>
@@ -935,106 +1208,106 @@
     </row>
     <row r="33" spans="1:3">
       <c r="A33" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B33" t="s">
         <v>44</v>
       </c>
       <c r="C33">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="34" spans="1:3">
       <c r="A34" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B34" t="s">
         <v>45</v>
       </c>
       <c r="C34">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="35" spans="1:3">
       <c r="A35" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B35" t="s">
         <v>46</v>
       </c>
       <c r="C35">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="36" spans="1:3">
       <c r="A36" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B36" t="s">
         <v>47</v>
       </c>
       <c r="C36">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="37" spans="1:3">
       <c r="A37" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="B37" t="s">
         <v>48</v>
       </c>
       <c r="C37">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="38" spans="1:3">
       <c r="A38" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="B38" t="s">
         <v>49</v>
       </c>
       <c r="C38">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="39" spans="1:3">
       <c r="A39" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="B39" t="s">
         <v>50</v>
       </c>
       <c r="C39">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="40" spans="1:3">
       <c r="A40" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="B40" t="s">
         <v>51</v>
       </c>
       <c r="C40">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="41" spans="1:3">
       <c r="A41" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B41" t="s">
         <v>52</v>
       </c>
       <c r="C41">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="42" spans="1:3">
       <c r="A42" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B42" t="s">
         <v>53</v>
@@ -1045,18 +1318,18 @@
     </row>
     <row r="43" spans="1:3">
       <c r="A43" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B43" t="s">
         <v>54</v>
       </c>
       <c r="C43">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="44" spans="1:3">
       <c r="A44" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B44" t="s">
         <v>55</v>
@@ -1067,18 +1340,18 @@
     </row>
     <row r="45" spans="1:3">
       <c r="A45" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B45" t="s">
         <v>56</v>
       </c>
       <c r="C45">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="46" spans="1:3">
       <c r="A46" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B46" t="s">
         <v>57</v>
@@ -1089,29 +1362,29 @@
     </row>
     <row r="47" spans="1:3">
       <c r="A47" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="B47" t="s">
         <v>58</v>
       </c>
       <c r="C47">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="48" spans="1:3">
       <c r="A48" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="B48" t="s">
         <v>59</v>
       </c>
       <c r="C48">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="49" spans="1:3">
       <c r="A49" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="B49" t="s">
         <v>60</v>
@@ -1122,40 +1395,40 @@
     </row>
     <row r="50" spans="1:3">
       <c r="A50" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="B50" t="s">
         <v>61</v>
       </c>
       <c r="C50">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="51" spans="1:3">
       <c r="A51" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="B51" t="s">
         <v>62</v>
       </c>
       <c r="C51">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="52" spans="1:3">
       <c r="A52" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="B52" t="s">
         <v>63</v>
       </c>
       <c r="C52">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="53" spans="1:3">
       <c r="A53" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="B53" t="s">
         <v>64</v>
@@ -1166,7 +1439,7 @@
     </row>
     <row r="54" spans="1:3">
       <c r="A54" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="B54" t="s">
         <v>65</v>
@@ -1177,24 +1450,1036 @@
     </row>
     <row r="55" spans="1:3">
       <c r="A55" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="B55" t="s">
         <v>66</v>
       </c>
       <c r="C55">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="56" spans="1:3">
       <c r="A56" t="s">
+        <v>7</v>
+      </c>
+      <c r="B56" t="s">
+        <v>7</v>
+      </c>
+      <c r="C56">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3">
+      <c r="A57" t="s">
+        <v>7</v>
+      </c>
+      <c r="B57" t="s">
+        <v>67</v>
+      </c>
+      <c r="C57">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3">
+      <c r="A58" t="s">
+        <v>7</v>
+      </c>
+      <c r="B58" t="s">
+        <v>68</v>
+      </c>
+      <c r="C58">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3">
+      <c r="A59" t="s">
+        <v>7</v>
+      </c>
+      <c r="B59" t="s">
+        <v>69</v>
+      </c>
+      <c r="C59">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3">
+      <c r="A60" t="s">
+        <v>7</v>
+      </c>
+      <c r="B60" t="s">
+        <v>70</v>
+      </c>
+      <c r="C60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3">
+      <c r="A61" t="s">
+        <v>7</v>
+      </c>
+      <c r="B61" t="s">
+        <v>71</v>
+      </c>
+      <c r="C61">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3">
+      <c r="A62" t="s">
+        <v>7</v>
+      </c>
+      <c r="B62" t="s">
+        <v>72</v>
+      </c>
+      <c r="C62">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3">
+      <c r="A63" t="s">
+        <v>7</v>
+      </c>
+      <c r="B63" t="s">
+        <v>73</v>
+      </c>
+      <c r="C63">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3">
+      <c r="A64" t="s">
+        <v>7</v>
+      </c>
+      <c r="B64" t="s">
+        <v>74</v>
+      </c>
+      <c r="C64">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3">
+      <c r="A65" t="s">
+        <v>7</v>
+      </c>
+      <c r="B65" t="s">
+        <v>75</v>
+      </c>
+      <c r="C65">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3">
+      <c r="A66" t="s">
+        <v>7</v>
+      </c>
+      <c r="B66" t="s">
+        <v>76</v>
+      </c>
+      <c r="C66">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3">
+      <c r="A67" t="s">
+        <v>7</v>
+      </c>
+      <c r="B67" t="s">
+        <v>77</v>
+      </c>
+      <c r="C67">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3">
+      <c r="A68" t="s">
+        <v>8</v>
+      </c>
+      <c r="B68" t="s">
+        <v>78</v>
+      </c>
+      <c r="C68">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3">
+      <c r="A69" t="s">
+        <v>8</v>
+      </c>
+      <c r="B69" t="s">
+        <v>79</v>
+      </c>
+      <c r="C69">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3">
+      <c r="A70" t="s">
+        <v>8</v>
+      </c>
+      <c r="B70" t="s">
+        <v>80</v>
+      </c>
+      <c r="C70">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3">
+      <c r="A71" t="s">
+        <v>8</v>
+      </c>
+      <c r="B71" t="s">
+        <v>81</v>
+      </c>
+      <c r="C71">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3">
+      <c r="A72" t="s">
+        <v>8</v>
+      </c>
+      <c r="B72" t="s">
+        <v>82</v>
+      </c>
+      <c r="C72">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3">
+      <c r="A73" t="s">
+        <v>8</v>
+      </c>
+      <c r="B73" t="s">
+        <v>83</v>
+      </c>
+      <c r="C73">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3">
+      <c r="A74" t="s">
+        <v>8</v>
+      </c>
+      <c r="B74" t="s">
+        <v>84</v>
+      </c>
+      <c r="C74">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3">
+      <c r="A75" t="s">
+        <v>8</v>
+      </c>
+      <c r="B75" t="s">
+        <v>85</v>
+      </c>
+      <c r="C75">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3">
+      <c r="A76" t="s">
+        <v>8</v>
+      </c>
+      <c r="B76" t="s">
+        <v>86</v>
+      </c>
+      <c r="C76">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3">
+      <c r="A77" t="s">
+        <v>8</v>
+      </c>
+      <c r="B77" t="s">
+        <v>87</v>
+      </c>
+      <c r="C77">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3">
+      <c r="A78" t="s">
+        <v>8</v>
+      </c>
+      <c r="B78" t="s">
+        <v>88</v>
+      </c>
+      <c r="C78">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3">
+      <c r="A79" t="s">
+        <v>8</v>
+      </c>
+      <c r="B79" t="s">
+        <v>89</v>
+      </c>
+      <c r="C79">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3">
+      <c r="A80" t="s">
+        <v>9</v>
+      </c>
+      <c r="B80" t="s">
+        <v>90</v>
+      </c>
+      <c r="C80">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3">
+      <c r="A81" t="s">
+        <v>9</v>
+      </c>
+      <c r="B81" t="s">
+        <v>91</v>
+      </c>
+      <c r="C81">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3">
+      <c r="A82" t="s">
+        <v>9</v>
+      </c>
+      <c r="B82" t="s">
+        <v>92</v>
+      </c>
+      <c r="C82">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3">
+      <c r="A83" t="s">
+        <v>9</v>
+      </c>
+      <c r="B83" t="s">
+        <v>93</v>
+      </c>
+      <c r="C83">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3">
+      <c r="A84" t="s">
+        <v>9</v>
+      </c>
+      <c r="B84" t="s">
+        <v>94</v>
+      </c>
+      <c r="C84">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3">
+      <c r="A85" t="s">
+        <v>9</v>
+      </c>
+      <c r="B85" t="s">
+        <v>95</v>
+      </c>
+      <c r="C85">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3">
+      <c r="A86" t="s">
+        <v>9</v>
+      </c>
+      <c r="B86" t="s">
+        <v>96</v>
+      </c>
+      <c r="C86">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3">
+      <c r="A87" t="s">
+        <v>9</v>
+      </c>
+      <c r="B87" t="s">
+        <v>97</v>
+      </c>
+      <c r="C87">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3">
+      <c r="A88" t="s">
+        <v>9</v>
+      </c>
+      <c r="B88" t="s">
+        <v>98</v>
+      </c>
+      <c r="C88">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3">
+      <c r="A89" t="s">
+        <v>9</v>
+      </c>
+      <c r="B89" t="s">
+        <v>99</v>
+      </c>
+      <c r="C89">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3">
+      <c r="A90" t="s">
+        <v>9</v>
+      </c>
+      <c r="B90" t="s">
+        <v>100</v>
+      </c>
+      <c r="C90">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3">
+      <c r="A91" t="s">
+        <v>9</v>
+      </c>
+      <c r="B91" t="s">
+        <v>101</v>
+      </c>
+      <c r="C91">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3">
+      <c r="A92" t="s">
+        <v>9</v>
+      </c>
+      <c r="B92" t="s">
+        <v>102</v>
+      </c>
+      <c r="C92">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3">
+      <c r="A93" t="s">
+        <v>9</v>
+      </c>
+      <c r="B93" t="s">
+        <v>103</v>
+      </c>
+      <c r="C93">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3">
+      <c r="A94" t="s">
+        <v>10</v>
+      </c>
+      <c r="B94" t="s">
+        <v>104</v>
+      </c>
+      <c r="C94">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3">
+      <c r="A95" t="s">
+        <v>10</v>
+      </c>
+      <c r="B95" t="s">
+        <v>105</v>
+      </c>
+      <c r="C95">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3">
+      <c r="A96" t="s">
+        <v>10</v>
+      </c>
+      <c r="B96" t="s">
+        <v>106</v>
+      </c>
+      <c r="C96">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3">
+      <c r="A97" t="s">
+        <v>10</v>
+      </c>
+      <c r="B97" t="s">
+        <v>107</v>
+      </c>
+      <c r="C97">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3">
+      <c r="A98" t="s">
+        <v>10</v>
+      </c>
+      <c r="B98" t="s">
+        <v>108</v>
+      </c>
+      <c r="C98">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3">
+      <c r="A99" t="s">
+        <v>10</v>
+      </c>
+      <c r="B99" t="s">
+        <v>109</v>
+      </c>
+      <c r="C99">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3">
+      <c r="A100" t="s">
+        <v>10</v>
+      </c>
+      <c r="B100" t="s">
+        <v>110</v>
+      </c>
+      <c r="C100">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3">
+      <c r="A101" t="s">
+        <v>10</v>
+      </c>
+      <c r="B101" t="s">
+        <v>111</v>
+      </c>
+      <c r="C101">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3">
+      <c r="A102" t="s">
+        <v>10</v>
+      </c>
+      <c r="B102" t="s">
+        <v>112</v>
+      </c>
+      <c r="C102">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3">
+      <c r="A103" t="s">
+        <v>10</v>
+      </c>
+      <c r="B103" t="s">
+        <v>113</v>
+      </c>
+      <c r="C103">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3">
+      <c r="A104" t="s">
+        <v>10</v>
+      </c>
+      <c r="B104" t="s">
+        <v>114</v>
+      </c>
+      <c r="C104">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3">
+      <c r="A105" t="s">
+        <v>10</v>
+      </c>
+      <c r="B105" t="s">
+        <v>115</v>
+      </c>
+      <c r="C105">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3">
+      <c r="A106" t="s">
+        <v>10</v>
+      </c>
+      <c r="B106" t="s">
+        <v>116</v>
+      </c>
+      <c r="C106">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3">
+      <c r="A107" t="s">
+        <v>10</v>
+      </c>
+      <c r="B107" t="s">
+        <v>117</v>
+      </c>
+      <c r="C107">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3">
+      <c r="A108" t="s">
+        <v>10</v>
+      </c>
+      <c r="B108" t="s">
+        <v>118</v>
+      </c>
+      <c r="C108">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3">
+      <c r="A109" t="s">
+        <v>11</v>
+      </c>
+      <c r="B109" t="s">
+        <v>119</v>
+      </c>
+      <c r="C109">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3">
+      <c r="A110" t="s">
+        <v>11</v>
+      </c>
+      <c r="B110" t="s">
+        <v>120</v>
+      </c>
+      <c r="C110">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3">
+      <c r="A111" t="s">
+        <v>11</v>
+      </c>
+      <c r="B111" t="s">
+        <v>121</v>
+      </c>
+      <c r="C111">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3">
+      <c r="A112" t="s">
+        <v>11</v>
+      </c>
+      <c r="B112" t="s">
+        <v>122</v>
+      </c>
+      <c r="C112">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3">
+      <c r="A113" t="s">
+        <v>11</v>
+      </c>
+      <c r="B113" t="s">
+        <v>123</v>
+      </c>
+      <c r="C113">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3">
+      <c r="A114" t="s">
+        <v>11</v>
+      </c>
+      <c r="B114" t="s">
+        <v>124</v>
+      </c>
+      <c r="C114">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3">
+      <c r="A115" t="s">
+        <v>11</v>
+      </c>
+      <c r="B115" t="s">
+        <v>125</v>
+      </c>
+      <c r="C115">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3">
+      <c r="A116" t="s">
+        <v>11</v>
+      </c>
+      <c r="B116" t="s">
+        <v>126</v>
+      </c>
+      <c r="C116">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3">
+      <c r="A117" t="s">
+        <v>11</v>
+      </c>
+      <c r="B117" t="s">
+        <v>127</v>
+      </c>
+      <c r="C117">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3">
+      <c r="A118" t="s">
+        <v>11</v>
+      </c>
+      <c r="B118" t="s">
+        <v>128</v>
+      </c>
+      <c r="C118">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3">
+      <c r="A119" t="s">
+        <v>11</v>
+      </c>
+      <c r="B119" t="s">
+        <v>129</v>
+      </c>
+      <c r="C119">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3">
+      <c r="A120" t="s">
+        <v>11</v>
+      </c>
+      <c r="B120" t="s">
+        <v>130</v>
+      </c>
+      <c r="C120">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3">
+      <c r="A121" t="s">
+        <v>11</v>
+      </c>
+      <c r="B121" t="s">
+        <v>131</v>
+      </c>
+      <c r="C121">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3">
+      <c r="A122" t="s">
+        <v>11</v>
+      </c>
+      <c r="B122" t="s">
+        <v>132</v>
+      </c>
+      <c r="C122">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3">
+      <c r="A123" t="s">
+        <v>11</v>
+      </c>
+      <c r="B123" t="s">
+        <v>133</v>
+      </c>
+      <c r="C123">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3">
+      <c r="A124" t="s">
+        <v>12</v>
+      </c>
+      <c r="B124" t="s">
+        <v>134</v>
+      </c>
+      <c r="C124">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3">
+      <c r="A125" t="s">
+        <v>12</v>
+      </c>
+      <c r="B125" t="s">
+        <v>135</v>
+      </c>
+      <c r="C125">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3">
+      <c r="A126" t="s">
+        <v>12</v>
+      </c>
+      <c r="B126" t="s">
+        <v>136</v>
+      </c>
+      <c r="C126">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3">
+      <c r="A127" t="s">
+        <v>12</v>
+      </c>
+      <c r="B127" t="s">
+        <v>137</v>
+      </c>
+      <c r="C127">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3">
+      <c r="A128" t="s">
+        <v>12</v>
+      </c>
+      <c r="B128" t="s">
+        <v>138</v>
+      </c>
+      <c r="C128">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3">
+      <c r="A129" t="s">
+        <v>12</v>
+      </c>
+      <c r="B129" t="s">
+        <v>139</v>
+      </c>
+      <c r="C129">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3">
+      <c r="A130" t="s">
+        <v>12</v>
+      </c>
+      <c r="B130" t="s">
+        <v>140</v>
+      </c>
+      <c r="C130">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3">
+      <c r="A131" t="s">
+        <v>12</v>
+      </c>
+      <c r="B131" t="s">
+        <v>141</v>
+      </c>
+      <c r="C131">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3">
+      <c r="A132" t="s">
+        <v>12</v>
+      </c>
+      <c r="B132" t="s">
+        <v>142</v>
+      </c>
+      <c r="C132">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3">
+      <c r="A133" t="s">
+        <v>12</v>
+      </c>
+      <c r="B133" t="s">
+        <v>143</v>
+      </c>
+      <c r="C133">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3">
+      <c r="A134" t="s">
+        <v>12</v>
+      </c>
+      <c r="B134" t="s">
+        <v>144</v>
+      </c>
+      <c r="C134">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3">
+      <c r="A135" t="s">
+        <v>12</v>
+      </c>
+      <c r="B135" t="s">
+        <v>145</v>
+      </c>
+      <c r="C135">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3">
+      <c r="A136" t="s">
         <v>13</v>
       </c>
-      <c r="B56" t="s">
-        <v>67</v>
-      </c>
-      <c r="C56">
-        <v>4</v>
+      <c r="B136" t="s">
+        <v>146</v>
+      </c>
+      <c r="C136">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3">
+      <c r="A137" t="s">
+        <v>13</v>
+      </c>
+      <c r="B137" t="s">
+        <v>147</v>
+      </c>
+      <c r="C137">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3">
+      <c r="A138" t="s">
+        <v>13</v>
+      </c>
+      <c r="B138" t="s">
+        <v>148</v>
+      </c>
+      <c r="C138">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3">
+      <c r="A139" t="s">
+        <v>13</v>
+      </c>
+      <c r="B139" t="s">
+        <v>149</v>
+      </c>
+      <c r="C139">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3">
+      <c r="A140" t="s">
+        <v>13</v>
+      </c>
+      <c r="B140" t="s">
+        <v>150</v>
+      </c>
+      <c r="C140">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="141" spans="1:3">
+      <c r="A141" t="s">
+        <v>13</v>
+      </c>
+      <c r="B141" t="s">
+        <v>151</v>
+      </c>
+      <c r="C141">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="142" spans="1:3">
+      <c r="A142" t="s">
+        <v>13</v>
+      </c>
+      <c r="B142" t="s">
+        <v>152</v>
+      </c>
+      <c r="C142">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="143" spans="1:3">
+      <c r="A143" t="s">
+        <v>13</v>
+      </c>
+      <c r="B143" t="s">
+        <v>153</v>
+      </c>
+      <c r="C143">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="144" spans="1:3">
+      <c r="A144" t="s">
+        <v>13</v>
+      </c>
+      <c r="B144" t="s">
+        <v>154</v>
+      </c>
+      <c r="C144">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="145" spans="1:3">
+      <c r="A145" t="s">
+        <v>13</v>
+      </c>
+      <c r="B145" t="s">
+        <v>155</v>
+      </c>
+      <c r="C145">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="146" spans="1:3">
+      <c r="A146" t="s">
+        <v>13</v>
+      </c>
+      <c r="B146" t="s">
+        <v>156</v>
+      </c>
+      <c r="C146">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="147" spans="1:3">
+      <c r="A147" t="s">
+        <v>13</v>
+      </c>
+      <c r="B147" t="s">
+        <v>157</v>
+      </c>
+      <c r="C147">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="148" spans="1:3">
+      <c r="A148" t="s">
+        <v>13</v>
+      </c>
+      <c r="B148" t="s">
+        <v>158</v>
+      </c>
+      <c r="C148">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>